<commit_message>
17 and 18 Aug Attendance
17 and 18 Aug Attendance
</commit_message>
<xml_diff>
--- a/B8-G1 Team_Everyday_Attendence.xlsx
+++ b/B8-G1 Team_Everyday_Attendence.xlsx
@@ -386,12 +386,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="G15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Informed</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -826,7 +922,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -834,11 +930,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1243,10 +1339,74 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>45155</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>45156</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2:A14"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2:A16"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:K1048576">
       <formula1>"PRESENT, ABSENT"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
9th and 11th Sept Attendance
9th and 11th Sept Attendance
</commit_message>
<xml_diff>
--- a/B8-G1 Team_Everyday_Attendence.xlsx
+++ b/B8-G1 Team_Everyday_Attendence.xlsx
@@ -2452,12 +2452,252 @@
         </r>
       </text>
     </comment>
+    <comment ref="D34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to work cant join </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to worl load cant join</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to work</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to work load</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -2895,7 +3135,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2903,11 +3143,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3911,10 +4151,80 @@
         <v>2</v>
       </c>
     </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>45178</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>45180</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2:A33"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2:A35"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:K1048576">
       <formula1>"PRESENT, ABSENT"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
10th and 11 Oct Attendance
10th and 11 Oct Attendance
</commit_message>
<xml_diff>
--- a/B8-G1 Team_Everyday_Attendence.xlsx
+++ b/B8-G1 Team_Everyday_Attendence.xlsx
@@ -3388,12 +3388,204 @@
         </r>
       </text>
     </comment>
+    <comment ref="B44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to some work</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Same</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Same</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to exam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Same</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Same</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -3831,7 +4023,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3839,11 +4031,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5162,10 +5354,80 @@
         <v>2</v>
       </c>
     </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>45209</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>1</v>
+      </c>
+      <c r="K44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>45210</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>1</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1</v>
+      </c>
+      <c r="J45" t="s">
+        <v>1</v>
+      </c>
+      <c r="K45" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2:A38 A40:A43"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2:A38 A40:A45"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:K1048576">
       <formula1>"PRESENT, ABSENT"</formula1>
     </dataValidation>

</xml_diff>